<commit_message>
Add ProsthoWolf backstory page and translations
</commit_message>
<xml_diff>
--- a/MultiLangComic/Excel翻譯_Extractosaurus_BS.xlsx
+++ b/MultiLangComic/Excel翻譯_Extractosaurus_BS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\GitHubTranslation\Risch315815.github.io\MultiLangComic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E82D68E-7D32-483A-B776-83BAB513A9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32648B0A-D14B-47F9-81F3-5A164CECF7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="2" xr2:uid="{0BB7FA42-6028-449D-B633-BAF7A0E05F3F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>en</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -447,57 +447,132 @@
     <t>th</t>
   </si>
   <si>
-    <t>It won't hurt at all after the local anesthesia~</t>
+    <t>I refuse.
+With your poor oral hygiene, your tooth would just decay until it fractures even if it is protected by a crown.</t>
   </si>
   <si>
-    <t>It won't hurt at all after the local anesthesia~</t>
+    <t>I refuse.
+With your poor oral hygiene, your tooth would just decay until it fractures even if it is protected by a crown.</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Nice~
-It went smoothly~</t>
+    <t>Hey!
+How dare you call my oral hygiene bad!</t>
   </si>
   <si>
-    <t>Nice~
-It went smoothly~</t>
+    <t>Hey!
+How dare you call my oral hygiene bad!</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>局所麻酔後も全然痛くないよ~</t>
+    <t>Please do not let you food drop onto the floor.</t>
   </si>
   <si>
-    <t>No dolerá en absoluto después de la anestesia local ~</t>
-  </si>
-  <si>
-    <t>Cela ne fera pas mal du tout après l’anesthésie locale ~</t>
-  </si>
-  <si>
-    <t>ไม่เจ็บเลยหลังจากดมยาสลบเฉพาะที่ ~</t>
-  </si>
-  <si>
-    <t>ナイス~
-スムーズに進みました~</t>
-  </si>
-  <si>
-    <t>Muy bien~
-Salió sin problemas ~</t>
-  </si>
-  <si>
-    <t>Gentil~
-Tout s’est bien passé~</t>
-  </si>
-  <si>
-    <t>ดี~
-มันราบรื่น~</t>
-  </si>
-  <si>
-    <t>我們很順利地
-拔起來囉~</t>
+    <t>Please do not let you food drop onto the floor.</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>打麻醉以後
-就不會痛囉~</t>
+    <t>You place your dental implant too shallow!</t>
+  </si>
+  <si>
+    <t>You place your dental implant too shallow!</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>The emergence profile of your crown is ugly.</t>
+  </si>
+  <si>
+    <t>The emergence profile of your crown is ugly.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>私は拒否します。
+口腔衛生状態が悪いと、歯冠で保護されていても、歯が骨折するまで虫歯になってしまいます。</t>
+  </si>
+  <si>
+    <t>Me niego.
+Con una mala higiene bucal, su diente simplemente se deterioraría hasta fracturarse, incluso si está protegido por una corona.</t>
+  </si>
+  <si>
+    <t>Je refuse.
+Avec votre mauvaise hygiène bucco-dentaire, votre dent ne ferait que se décomposer jusqu’à ce qu’elle se fracture, même si elle est protégée par une couronne.</t>
+  </si>
+  <si>
+    <t>ฉันปฏิเสธ
+ด้วยสุขอนามัยในช่องปากที่ไม่ดีฟันของคุณจะผุจนหักแม้ว่าจะได้รับการปกป้องด้วยครอบฟันก็ตาม</t>
+  </si>
+  <si>
+    <t>ねえ！
+私の口腔衛生を悪いと呼ぶなんて!</t>
+  </si>
+  <si>
+    <t>¡Eh!
+¡Cómo te atreves a decir que mi higiene bucal es mala!</t>
+  </si>
+  <si>
+    <t>Hé!
+Comment osez-vous dire que mon hygiène bucco-dentaire est mauvaise !</t>
+  </si>
+  <si>
+    <t>หวัดดี!
+คุณกล้าเรียกสุขอนามัยในช่องปากของฉันว่าไม่ดีได้อย่างไร!</t>
+  </si>
+  <si>
+    <t>食べ物を床に落とさないでください。</t>
+  </si>
+  <si>
+    <t>Por favor, no deje que la comida caiga al suelo.</t>
+  </si>
+  <si>
+    <t>Veuillez ne pas laisser tomber votre nourriture sur le sol.</t>
+  </si>
+  <si>
+    <t>โปรดอย่าปล่อยให้อาหารหล่นลงบนพื้น</t>
+  </si>
+  <si>
+    <t>歯科インプラントを浅くしすぎます!</t>
+  </si>
+  <si>
+    <t>¡Colocas tu implante dental demasiado poco profundo!</t>
+  </si>
+  <si>
+    <t>Vous placez votre implant dentaire trop peu profond !</t>
+  </si>
+  <si>
+    <t>คุณวางรากฟันเทียมตื้นเกินไป!</t>
+  </si>
+  <si>
+    <t>あなたの王冠の出現プロファイルは醜いです。</t>
+  </si>
+  <si>
+    <t>El perfil de emergencia de su corona es feo.</t>
+  </si>
+  <si>
+    <t>Le profil d’émergence de votre couronne est moche.</t>
+  </si>
+  <si>
+    <t>โปรไฟล์การเกิดขึ้นของมงกุฎของคุณน่าเกลียด</t>
+  </si>
+  <si>
+    <t>我拒絕。
+口腔衛生這麼差，做了牙冠也是蛀掉。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>欸！
+說誰的口腔衛生差呢！?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>請不要讓食物掉到診間地板。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>你植的太淺了！</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>是你的 emergence profile 醜~</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -8074,7 +8149,7 @@
   <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+      <selection activeCell="A2" sqref="A2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.149999999999999"/>
@@ -8115,7 +8190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30.75">
+    <row r="2" spans="1:8" ht="92.25">
       <c r="A2" s="16" t="s">
         <v>36</v>
       </c>
@@ -8125,30 +8200,36 @@
       </c>
       <c r="C2" s="9" t="str">
         <f>_xlfn.TRANSLATE($A2,$B2,C$1)</f>
-        <v>It won't hurt at all after the local anesthesia~</v>
+        <v>I refuse.
+With your poor oral hygiene, your tooth would just decay until it fractures even if it is protected by a crown.</v>
       </c>
       <c r="D2" s="18" t="str">
         <f t="shared" ref="D2:H13" si="0">_xlfn.TRANSLATE($A2,$B2,D$1)</f>
-        <v>局部麻醉后一點都不會疼~</v>
+        <v>我拒絕。
+由於口腔衛生不佳，即使有牙冠保護，您的牙齒也會腐爛直到斷裂。</v>
       </c>
       <c r="E2" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>局所麻酔後も全然痛くないよ~</v>
+        <v>私は拒否します。
+口腔衛生状態が悪いと、歯冠で保護されていても、歯が骨折するまで虫歯になってしまいます。</v>
       </c>
       <c r="F2" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>No dolerá en absoluto después de la anestesia local ~</v>
+        <v>Me niego.
+Con una mala higiene bucal, su diente simplemente se deterioraría hasta fracturarse, incluso si está protegido por una corona.</v>
       </c>
       <c r="G2" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>Cela ne fera pas mal du tout après l’anesthésie locale ~</v>
+        <v>Je refuse.
+Avec votre mauvaise hygiène bucco-dentaire, votre dent ne ferait que se décomposer jusqu’à ce qu’elle se fracture, même si elle est protégée par une couronne.</v>
       </c>
       <c r="H2" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>ไม่เจ็บเลยหลังจากดมยาสลบเฉพาะที่ ~</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30.75">
+        <v>ฉันปฏิเสธ
+ด้วยสุขอนามัยในช่องปากที่ไม่ดีฟันของคุณจะผุจนหักแม้ว่าจะได้รับการปกป้องด้วยครอบฟันก็ตาม</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="46.15">
       <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
@@ -8158,126 +8239,132 @@
       </c>
       <c r="C3" s="9" t="str">
         <f t="shared" ref="C3:C13" si="2">_xlfn.TRANSLATE($A3,$B3,C$1)</f>
-        <v>Nice~
-It went smoothly~</v>
+        <v>Hey!
+How dare you call my oral hygiene bad!</v>
       </c>
       <c r="D3" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>好~
-一切順利~</v>
+        <v>嘿！
+你怎麼敢說我的口腔衛生不好！</v>
       </c>
       <c r="E3" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>ナイス~
-スムーズに進みました~</v>
+        <v>ねえ！
+私の口腔衛生を悪いと呼ぶなんて!</v>
       </c>
       <c r="F3" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Muy bien~
-Salió sin problemas ~</v>
+        <v>¡Eh!
+¡Cómo te atreves a decir que mi higiene bucal es mala!</v>
       </c>
       <c r="G3" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>Gentil~
-Tout s’est bien passé~</v>
+        <v>Hé!
+Comment osez-vous dire que mon hygiène bucco-dentaire est mauvaise !</v>
       </c>
       <c r="H3" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>ดี~
-มันราบรื่น~</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="16"/>
+        <v>หวัดดี!
+คุณกล้าเรียกสุขอนามัยในช่องปากของฉันว่าไม่ดีได้อย่างไร!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30.75">
+      <c r="A4" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>en</v>
       </c>
       <c r="C4" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Please do not let you food drop onto the floor.</v>
       </c>
       <c r="D4" s="18" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>請不要讓您的食物掉到地板上。</v>
       </c>
       <c r="E4" s="19" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>食べ物を床に落とさないでください。</v>
       </c>
       <c r="F4" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Por favor, no deje que la comida caiga al suelo.</v>
       </c>
       <c r="G4" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Veuillez ne pas laisser tomber votre nourriture sur le sol.</v>
       </c>
       <c r="H4" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="16"/>
+        <v>โปรดอย่าปล่อยให้อาหารหล่นลงบนพื้น</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30.75">
+      <c r="A5" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>en</v>
       </c>
       <c r="C5" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>You place your dental implant too shallow!</v>
       </c>
       <c r="D5" s="18" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>你把種植牙放得太淺了！</v>
       </c>
       <c r="E5" s="19" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>歯科インプラントを浅くしすぎます!</v>
       </c>
       <c r="F5" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>¡Colocas tu implante dental demasiado poco profundo!</v>
       </c>
       <c r="G5" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Vous placez votre implant dentaire trop peu profond !</v>
       </c>
       <c r="H5" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="16"/>
+        <v>คุณวางรากฟันเทียมตื้นเกินไป!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30.75">
+      <c r="A6" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>en</v>
       </c>
       <c r="C6" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>The emergence profile of your crown is ugly.</v>
       </c>
       <c r="D6" s="18" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>你的牙冠的出現輪廓很醜陋。</v>
       </c>
       <c r="E6" s="19" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>あなたの王冠の出現プロファイルは醜いです。</v>
       </c>
       <c r="F6" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>El perfil de emergencia de su corona es feo.</v>
       </c>
       <c r="G6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Le profil d’émergence de votre couronne est moche.</v>
       </c>
       <c r="H6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>โปรไฟล์การเกิดขึ้นของมงกุฎของคุณน่าเกลียด</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -14089,7 +14176,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.149999999999999"/>
@@ -14126,7 +14213,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32.25">
+    <row r="2" spans="1:8" ht="48.4">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -14137,19 +14224,19 @@
         <v>35</v>
       </c>
       <c r="D2" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32.25">
@@ -14163,24 +14250,98 @@
         <v>37</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="D8" s="21"/>

</xml_diff>